<commit_message>
Ajout du controleur, du model et d'une manière de naviguer entre les menus autre que enter et échape.
</commit_message>
<xml_diff>
--- a/Log de tâche.xlsx
+++ b/Log de tâche.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="2F14059B8F6B36D421CB6D186C1403506DED38A2" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{8859D0E3-FAC8-4278-95D3-45E8DECE82D0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Membre1" sheetId="1" r:id="rId1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -66,12 +67,21 @@
   </si>
   <si>
     <t>Remplir les logs</t>
+  </si>
+  <si>
+    <t>30min</t>
+  </si>
+  <si>
+    <t>Création du contrôle/model, ajout de la navigation entre les menus</t>
+  </si>
+  <si>
+    <t>La première fois que j'utilise un dictionnaire, le find_if et des expressions lambda.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -210,6 +220,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -219,7 +230,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,30 +567,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" customWidth="1"/>
-    <col min="3" max="3" width="28.5546875" customWidth="1"/>
-    <col min="4" max="4" width="42.88671875" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="11"/>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="12"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -594,7 +604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>43031</v>
       </c>
@@ -608,8 +618,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="12">
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
         <v>43031</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -622,8 +632,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="12">
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
         <v>43031</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -636,8 +646,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="12">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
         <v>43031</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -648,145 +658,153 @@
       </c>
       <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>43031</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="8"/>
@@ -802,30 +820,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13:F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" customWidth="1"/>
-    <col min="3" max="3" width="28.5546875" customWidth="1"/>
-    <col min="4" max="4" width="42.88671875" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="11"/>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="12"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -839,169 +857,169 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="8"/>

</xml_diff>

<commit_message>
Implementation des singletons, de split(non testé) et de l'authentification (non testé)
</commit_message>
<xml_diff>
--- a/Log de tâche.xlsx
+++ b/Log de tâche.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="9" documentId="2F14059B8F6B36D421CB6D186C1403506DED38A2" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{ECDC060D-6AF4-48BD-BE1C-5F100E3A2A15}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="2F14059B8F6B36D421CB6D186C1403506DED38A2" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{9D1BAF8F-1FD1-4810-8602-33D18C934844}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -78,13 +78,31 @@
     <t>La première fois que j'utilise un dictionnaire, le find_if et des expressions lambda.</t>
   </si>
   <si>
-    <t>2017-1024</t>
-  </si>
-  <si>
     <t>Création SceneGestionCompte</t>
   </si>
   <si>
     <t>Savoir comment organiser les menus.</t>
+  </si>
+  <si>
+    <t>Mise au point de la navigation entre les menus</t>
+  </si>
+  <si>
+    <t>Le code de la navigation fonctionnait que si un textbox était actif.</t>
+  </si>
+  <si>
+    <t>Implementation des singletons</t>
+  </si>
+  <si>
+    <t>Le delete doit être fais à l'extérieur par une méthode static du singleton</t>
+  </si>
+  <si>
+    <t>40min</t>
+  </si>
+  <si>
+    <t>Il n'y a pas de méthode de split dans la librairie standard.</t>
+  </si>
+  <si>
+    <t>Implementation de l'authentification non testé et d'une méthode split non testé.</t>
   </si>
 </sst>
 </file>
@@ -580,7 +598,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -682,36 +700,60 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>20</v>
+      <c r="A8" s="9">
+        <v>43032</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="8" t="s">
+    </row>
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="9">
+        <v>43032</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
+      <c r="D9" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="9">
+        <v>43032</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="9">
+        <v>43032</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>

</xml_diff>

<commit_message>
Création des tests pour Modele::Split, Modele::AuthentifierUtilisateur, Controle::AuthentifierUtilisateur
</commit_message>
<xml_diff>
--- a/Log de tâche.xlsx
+++ b/Log de tâche.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="23" documentId="2F14059B8F6B36D421CB6D186C1403506DED38A2" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{9D1BAF8F-1FD1-4810-8602-33D18C934844}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="2F14059B8F6B36D421CB6D186C1403506DED38A2" xr6:coauthVersionLast="23" xr6:coauthVersionMax="23" xr10:uidLastSave="{6E28D48E-D194-427A-8068-028CECE9578D}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -96,13 +96,22 @@
     <t>Le delete doit être fais à l'extérieur par une méthode static du singleton</t>
   </si>
   <si>
-    <t>40min</t>
-  </si>
-  <si>
-    <t>Il n'y a pas de méthode de split dans la librairie standard.</t>
-  </si>
-  <si>
     <t>Implementation de l'authentification non testé et d'une méthode split non testé.</t>
+  </si>
+  <si>
+    <t>45min</t>
+  </si>
+  <si>
+    <t>1h45min</t>
+  </si>
+  <si>
+    <t>Tester Authentification et Split</t>
+  </si>
+  <si>
+    <t>Il n'y a pas de méthode de split/explode dans la librairie standard.</t>
+  </si>
+  <si>
+    <t>Des fois les tests ne compiles pas à cause qu'il ne trouve pas certains fichiers .obj, mais en rebuildant il marche… Defois les modifications ne sont pas prises en compte. On doit faire rouler le teste 2 fois. L'ajout de dépendance externe combiner avec le problème des échecs de compilation aléatoire... La position d'un fichier en rapport avec le ProjetTest combiner avec les modifications non prises en compte.</t>
   </si>
 </sst>
 </file>
@@ -597,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -746,20 +755,28 @@
         <v>43032</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="D11" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="9">
+        <v>43033</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
+      <c r="C12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
@@ -883,7 +900,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13:F14"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>